<commit_message>
Added neew excel with 10 numbers contct
</commit_message>
<xml_diff>
--- a/public/CMC_import_Template_v1.xlsx
+++ b/public/CMC_import_Template_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\Sanju Space\Web Applications\EMS\EMS-Frontend\Qubinest-Frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F97E9ED-B649-48F8-A31C-497E2F7EFB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36857F8D-FCD7-4EF3-B95D-A05C147B7ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1CE338C7-D65B-4040-912F-A34C5F7D4BB1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>name</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>preRegisteredAmount</t>
-  </si>
-  <si>
-    <t>ww</t>
   </si>
 </sst>
 </file>
@@ -452,13 +449,14 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
@@ -14023,9 +14021,7 @@
       <c r="A967" s="1"/>
       <c r="B967" s="1"/>
       <c r="C967" s="1"/>
-      <c r="D967" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="D967" s="1"/>
       <c r="E967" s="1"/>
       <c r="F967" s="1"/>
       <c r="G967" s="1"/>
@@ -14498,7 +14494,12 @@
       <c r="L1000" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="aF20XkFjSkKC2ekpNjw0DQ+mTBJMl6FRl1ylr+3qLpgmOH3WeDirxpcEAYgCtbhYTXww+9MlO2HwIzjhWfP5hQ==" saltValue="Kp27B/UxdLSaonOR1aFW8w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xtDL1829kFGDsFobreDgtBNNtJmMevovJoe1/wQGAU/BMCfdFljfJj1UTU1+q8VOp/J0Xk6bTe025cDINVhqIg==" saltValue="IB2jtbVNYTKxirPEhkiOdw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataValidations xWindow="112" yWindow="284" count="1">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Add 10 numbers only" sqref="B2:B1000" xr:uid="{B1C691AF-C348-4733-9D40-C22AC02D2F20}">
+      <formula1>10</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>